<commit_message>
fix: fixing excel format bug
</commit_message>
<xml_diff>
--- a/iphone_price.xlsx
+++ b/iphone_price.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,338 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Apple iPhone 13</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>8249000</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>113K</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Apple iPhone 15 Plus</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>13499000</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Apple iPhone 15</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>11249000</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>911</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Apple iPhone 16</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>14999000</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Apple iPhone 13</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>8249000</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>62K</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Apple iPhone 16</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>14999000</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Apple iPhone 15</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>13749000</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>658</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Apple iPhone 13 128 GB</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>8249000</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>777</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Apple iPhone 16</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>14998000</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Apple iPhone 15 128 GB</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11249000</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Apple iPhone 17</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>17249000</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>236</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Apple iPhone 15</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11249000</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>IPhone 17 Pro 17 Pro max 17 Air 16 16E 15 14 plus 13 12 11 Pro Promax X Xs Xr Xsmax New Tempered SUPERFIT Auto Install Anti SPY PRIVACY - HITAM Temperd Super Fit Instal Antigores Gores Screen Protector Tempred Glass Kaca Easy 4g 5g s Liquid Black Gelap</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>27256</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Apple iPhone 17 Pro Max</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>25749000</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>683</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Apple iPhone 16</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>14749000</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Apple iPhone 17 Pro</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>23749000</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>253</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>TELEPHONE IP PHONE CISCO 7942G NEW BERGARANSI</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>510000</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Apple iPhone 17 Pro</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>23749000</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Apple iPhone 14</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>9749000</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>679</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Apple iPhone 16e</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11749000</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>